<commit_message>
Update Nalco PDF (2025-08-15 04:03:20 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,27 +487,55 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D3" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -516,6 +544,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-08-21 03:50:54 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,42 +500,70 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D4" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -545,6 +573,7 @@
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-08-28 06:48:08 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,42 +528,70 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D5" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -574,6 +602,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-09-02 06:49:07 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,42 +556,70 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D6" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -603,6 +631,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-09-17 06:47:19 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,42 +584,70 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D7" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -632,6 +660,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-09-22 13:04:11 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,42 +612,70 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D8" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -661,6 +689,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-09-25 06:47:52 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,42 +640,70 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>ALUMINIUM INGOT</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>IE07</t>
         </is>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D9" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -690,6 +718,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-09-30 03:46:10 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,42 +668,70 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="F10" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -719,6 +747,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-10-04 06:43:17 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,42 +696,70 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F10" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -748,6 +776,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F10" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-10-09 06:48:28 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,42 +724,70 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -777,6 +805,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F10" r:id="rId9"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-10-14 06:47:18 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,42 +752,70 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E12" s="3" t="inlineStr">
+      <c r="E13" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="F13" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -806,6 +834,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F10" r:id="rId9"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F11" r:id="rId10"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F12" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-10-17 06:46:44 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,42 +780,70 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E13" s="3" t="inlineStr">
+      <c r="E14" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="F14" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -835,6 +863,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F11" r:id="rId10"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F12" r:id="rId11"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F13" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-10-25 03:47:18 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,42 +808,70 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E15" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F14" s="3" t="inlineStr">
+      <c r="F15" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -864,6 +892,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F12" r:id="rId11"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F13" r:id="rId12"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F14" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-10-30 06:48:50 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,42 +836,70 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E15" s="3" t="inlineStr">
+      <c r="E16" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F15" s="3" t="inlineStr">
+      <c r="F16" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -893,6 +921,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F13" r:id="rId12"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F14" r:id="rId13"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F15" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco PDF (2025-11-04 06:49:53 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
@@ -500,22 +500,22 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
@@ -528,22 +528,22 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
@@ -556,22 +556,22 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
@@ -612,22 +612,22 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
@@ -640,22 +640,22 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
@@ -668,22 +668,22 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
@@ -724,22 +724,22 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
@@ -752,22 +752,22 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
@@ -780,22 +780,22 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
@@ -808,22 +808,22 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
@@ -836,22 +836,22 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
@@ -864,42 +864,70 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>269.45</v>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>15-08-2025</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="3" t="inlineStr">
-        <is>
-          <t>ALUMINIUM INGOT</t>
-        </is>
-      </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>IE07</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
         <v>268.25</v>
       </c>
-      <c r="E16" s="3" t="inlineStr">
+      <c r="E17" s="3" t="inlineStr">
         <is>
           <t>07-08-2025</t>
         </is>
       </c>
-      <c r="F16" s="3" t="inlineStr">
+      <c r="F17" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -922,6 +950,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F14" r:id="rId13"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F15" r:id="rId14"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F16" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-06 03:57:50 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -622,23 +622,23 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -682,23 +682,23 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -832,23 +832,23 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1072,23 +1072,23 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1162,23 +1162,23 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1312,23 +1312,23 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3180,6 +3180,36 @@
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D92" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F92" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3277,6 +3307,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F89" r:id="rId88"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F90" r:id="rId89"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F91" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F92" r:id="rId91"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-07 03:52:58 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -652,23 +652,23 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -712,23 +712,23 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -862,23 +862,23 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1102,23 +1102,23 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1192,23 +1192,23 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1342,23 +1342,23 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3210,6 +3210,36 @@
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D93" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E93" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F93" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3308,6 +3338,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F90" r:id="rId89"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F91" r:id="rId90"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F92" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F93" r:id="rId92"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-08 03:48:20 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -682,23 +682,23 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -742,23 +742,23 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -892,23 +892,23 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1132,23 +1132,23 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1222,23 +1222,23 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1372,23 +1372,23 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3240,6 +3240,36 @@
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D94" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E94" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F94" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3339,6 +3369,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F91" r:id="rId90"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F92" r:id="rId91"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F93" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F94" r:id="rId93"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-09 03:54:20 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -712,23 +712,23 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -772,23 +772,23 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -922,23 +922,23 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1162,23 +1162,23 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1252,23 +1252,23 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3270,6 +3270,36 @@
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D95" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E95" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F95" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3370,6 +3400,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F92" r:id="rId91"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F93" r:id="rId92"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F94" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F95" r:id="rId94"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-10 04:00:22 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -742,23 +742,23 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -802,23 +802,23 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -952,23 +952,23 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1192,23 +1192,23 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1282,23 +1282,23 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3300,6 +3300,36 @@
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D96" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E96" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F96" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3401,6 +3431,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F93" r:id="rId92"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F94" r:id="rId93"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F95" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F96" r:id="rId95"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-11 03:55:59 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -772,23 +772,23 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -832,23 +832,23 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -982,23 +982,23 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1222,23 +1222,23 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1312,23 +1312,23 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3330,6 +3330,36 @@
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D97" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E97" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F97" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3432,6 +3462,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F94" r:id="rId93"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F95" r:id="rId94"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F96" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F97" r:id="rId96"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-12 03:54:49 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -802,23 +802,23 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -862,23 +862,23 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1012,23 +1012,23 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1252,23 +1252,23 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1342,23 +1342,23 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3360,6 +3360,36 @@
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D98" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E98" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F98" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3463,6 +3493,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F95" r:id="rId94"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F96" r:id="rId95"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F97" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F98" r:id="rId97"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-13 03:58:27 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -832,23 +832,23 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -892,23 +892,23 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1042,23 +1042,23 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1282,23 +1282,23 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1372,23 +1372,23 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3390,6 +3390,36 @@
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D99" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E99" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F99" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3494,6 +3524,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F96" r:id="rId95"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F97" r:id="rId96"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F98" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F99" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-14 03:55:59 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -862,23 +862,23 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -922,23 +922,23 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1072,23 +1072,23 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1312,23 +1312,23 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3420,6 +3420,36 @@
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B100" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C100" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D100" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F100" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3525,6 +3555,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F97" r:id="rId96"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F98" r:id="rId97"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F99" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F100" r:id="rId99"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-15 03:50:03 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -892,23 +892,23 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -952,23 +952,23 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1102,23 +1102,23 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1342,23 +1342,23 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3450,6 +3450,36 @@
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D101" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E101" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3556,6 +3586,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F98" r:id="rId97"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F99" r:id="rId98"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F100" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F101" r:id="rId100"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-16 03:59:18 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -922,23 +922,23 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -982,23 +982,23 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1132,23 +1132,23 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1372,23 +1372,23 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3480,6 +3480,36 @@
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B102" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D102" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F102" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3587,6 +3617,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F99" r:id="rId98"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F100" r:id="rId99"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F101" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F102" r:id="rId101"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-17 03:59:14 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -952,23 +952,23 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1012,23 +1012,23 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1162,23 +1162,23 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3510,6 +3510,36 @@
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D103" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E103" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F103" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3618,6 +3648,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F100" r:id="rId99"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F101" r:id="rId100"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F102" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F103" r:id="rId102"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-18 03:54:54 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -982,23 +982,23 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1042,23 +1042,23 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1192,23 +1192,23 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3322,23 +3322,23 @@
         </is>
       </c>
       <c r="D96" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3540,6 +3540,36 @@
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D104" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E104" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F104" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3649,6 +3679,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F101" r:id="rId100"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F102" r:id="rId101"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F103" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F104" r:id="rId103"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-19 03:54:40 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1012,23 +1012,23 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1072,23 +1072,23 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1222,23 +1222,23 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3352,23 +3352,23 @@
         </is>
       </c>
       <c r="D97" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3570,6 +3570,36 @@
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D105" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E105" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F105" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3680,6 +3710,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F102" r:id="rId101"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F103" r:id="rId102"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F104" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F105" r:id="rId104"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-20 03:53:26 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1042,23 +1042,23 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1102,23 +1102,23 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1252,23 +1252,23 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3382,23 +3382,23 @@
         </is>
       </c>
       <c r="D98" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3600,6 +3600,36 @@
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D106" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E106" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F106" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3711,6 +3741,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F103" r:id="rId102"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F104" r:id="rId103"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F105" r:id="rId104"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F106" r:id="rId105"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-21 03:53:08 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1072,23 +1072,23 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1132,23 +1132,23 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1282,23 +1282,23 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3412,23 +3412,23 @@
         </is>
       </c>
       <c r="D99" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3630,6 +3630,36 @@
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D107" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E107" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3742,6 +3772,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F104" r:id="rId103"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F105" r:id="rId104"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F106" r:id="rId105"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F107" r:id="rId106"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-22 03:49:18 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1102,23 +1102,23 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1162,23 +1162,23 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1312,23 +1312,23 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3442,23 +3442,23 @@
         </is>
       </c>
       <c r="D100" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3660,6 +3660,36 @@
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B108" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D108" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E108" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F108" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3773,6 +3803,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F105" r:id="rId104"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F106" r:id="rId105"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F107" r:id="rId106"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F108" r:id="rId107"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-23 04:07:49 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1132,23 +1132,23 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1192,23 +1192,23 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1342,23 +1342,23 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3472,23 +3472,23 @@
         </is>
       </c>
       <c r="D101" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3690,6 +3690,36 @@
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D109" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E109" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F109" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3804,6 +3834,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F106" r:id="rId105"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F107" r:id="rId106"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F108" r:id="rId107"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F109" r:id="rId108"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-24 04:07:42 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1162,23 +1162,23 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1222,23 +1222,23 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1372,23 +1372,23 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3322,23 +3322,23 @@
         </is>
       </c>
       <c r="D96" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3502,23 +3502,23 @@
         </is>
       </c>
       <c r="D102" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3720,6 +3720,36 @@
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B110" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C110" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D110" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E110" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3835,6 +3865,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F107" r:id="rId106"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F108" r:id="rId107"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F109" r:id="rId108"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F110" r:id="rId109"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-25 03:58:44 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1192,23 +1192,23 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1252,23 +1252,23 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3352,23 +3352,23 @@
         </is>
       </c>
       <c r="D97" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3532,23 +3532,23 @@
         </is>
       </c>
       <c r="D103" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3750,6 +3750,36 @@
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B111" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D111" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E111" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F111" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3866,6 +3896,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F108" r:id="rId107"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F109" r:id="rId108"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F110" r:id="rId109"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F111" r:id="rId110"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-26 03:58:17 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1222,23 +1222,23 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1282,23 +1282,23 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3382,23 +3382,23 @@
         </is>
       </c>
       <c r="D98" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3562,23 +3562,23 @@
         </is>
       </c>
       <c r="D104" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3780,6 +3780,36 @@
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B112" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C112" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D112" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E112" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F112" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3897,6 +3927,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F109" r:id="rId108"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F110" r:id="rId109"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F111" r:id="rId110"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F112" r:id="rId111"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-27 03:54:58 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1252,23 +1252,23 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1312,23 +1312,23 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3412,23 +3412,23 @@
         </is>
       </c>
       <c r="D99" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3592,23 +3592,23 @@
         </is>
       </c>
       <c r="D105" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3810,6 +3810,36 @@
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B113" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D113" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E113" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F113" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3928,6 +3958,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F110" r:id="rId109"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F111" r:id="rId110"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F112" r:id="rId111"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F113" r:id="rId112"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-28 03:54:44 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1282,23 +1282,23 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1342,23 +1342,23 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3442,23 +3442,23 @@
         </is>
       </c>
       <c r="D100" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3622,23 +3622,23 @@
         </is>
       </c>
       <c r="D106" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3840,6 +3840,36 @@
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B114" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C114" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D114" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E114" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F114" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3959,6 +3989,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F111" r:id="rId110"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F112" r:id="rId111"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F113" r:id="rId112"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F114" r:id="rId113"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-29 03:54:18 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1312,23 +1312,23 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1372,23 +1372,23 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3472,23 +3472,23 @@
         </is>
       </c>
       <c r="D101" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3652,23 +3652,23 @@
         </is>
       </c>
       <c r="D107" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3870,6 +3870,36 @@
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B115" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D115" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E115" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F115" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -3990,6 +4020,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F112" r:id="rId111"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F113" r:id="rId112"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F114" r:id="rId113"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F115" r:id="rId114"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-11-30 04:08:28 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1342,23 +1342,23 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3502,23 +3502,23 @@
         </is>
       </c>
       <c r="D102" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3682,23 +3682,23 @@
         </is>
       </c>
       <c r="D108" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3900,6 +3900,36 @@
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B116" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C116" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D116" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E116" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F116" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4021,6 +4051,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F113" r:id="rId112"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F114" r:id="rId113"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F115" r:id="rId114"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F116" r:id="rId115"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-01 04:33:24 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1372,23 +1372,23 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3322,23 +3322,23 @@
         </is>
       </c>
       <c r="D96" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3532,23 +3532,23 @@
         </is>
       </c>
       <c r="D103" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3712,23 +3712,23 @@
         </is>
       </c>
       <c r="D109" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3930,6 +3930,36 @@
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B117" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C117" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D117" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E117" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F117" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4052,6 +4082,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F114" r:id="rId113"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F115" r:id="rId114"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F116" r:id="rId115"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F117" r:id="rId116"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-02 04:02:46 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3352,23 +3352,23 @@
         </is>
       </c>
       <c r="D97" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3562,23 +3562,23 @@
         </is>
       </c>
       <c r="D104" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3742,23 +3742,23 @@
         </is>
       </c>
       <c r="D110" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3960,6 +3960,36 @@
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B118" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C118" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D118" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E118" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F118" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4083,6 +4113,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F115" r:id="rId114"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F116" r:id="rId115"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F117" r:id="rId116"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F118" r:id="rId117"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-02 06:53:32 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -502,16 +502,16 @@
         </is>
       </c>
       <c r="D2" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -532,16 +532,16 @@
         </is>
       </c>
       <c r="D3" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="D4" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -592,16 +592,16 @@
         </is>
       </c>
       <c r="D5" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -622,16 +622,16 @@
         </is>
       </c>
       <c r="D6" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -652,16 +652,16 @@
         </is>
       </c>
       <c r="D7" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -682,16 +682,16 @@
         </is>
       </c>
       <c r="D8" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="D9" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -742,16 +742,16 @@
         </is>
       </c>
       <c r="D10" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -772,16 +772,16 @@
         </is>
       </c>
       <c r="D11" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -802,16 +802,16 @@
         </is>
       </c>
       <c r="D12" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -832,16 +832,16 @@
         </is>
       </c>
       <c r="D13" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -862,16 +862,16 @@
         </is>
       </c>
       <c r="D14" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -892,16 +892,16 @@
         </is>
       </c>
       <c r="D15" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -922,16 +922,16 @@
         </is>
       </c>
       <c r="D16" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -952,16 +952,16 @@
         </is>
       </c>
       <c r="D17" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -982,16 +982,16 @@
         </is>
       </c>
       <c r="D18" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1012,16 +1012,16 @@
         </is>
       </c>
       <c r="D19" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1042,16 +1042,16 @@
         </is>
       </c>
       <c r="D20" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1072,16 +1072,16 @@
         </is>
       </c>
       <c r="D21" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1102,16 +1102,16 @@
         </is>
       </c>
       <c r="D22" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1132,16 +1132,16 @@
         </is>
       </c>
       <c r="D23" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1162,16 +1162,16 @@
         </is>
       </c>
       <c r="D24" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1192,16 +1192,16 @@
         </is>
       </c>
       <c r="D25" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1222,16 +1222,16 @@
         </is>
       </c>
       <c r="D26" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1252,16 +1252,16 @@
         </is>
       </c>
       <c r="D27" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1282,16 +1282,16 @@
         </is>
       </c>
       <c r="D28" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1312,16 +1312,16 @@
         </is>
       </c>
       <c r="D29" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1342,16 +1342,16 @@
         </is>
       </c>
       <c r="D30" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
@@ -1372,16 +1372,16 @@
         </is>
       </c>
       <c r="D31" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-03 04:00:59 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1402,23 +1402,23 @@
         </is>
       </c>
       <c r="D32" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3382,23 +3382,23 @@
         </is>
       </c>
       <c r="D98" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3592,23 +3592,23 @@
         </is>
       </c>
       <c r="D105" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3772,23 +3772,23 @@
         </is>
       </c>
       <c r="D111" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3990,6 +3990,36 @@
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B119" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C119" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D119" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E119" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F119" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4114,6 +4144,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F116" r:id="rId115"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F117" r:id="rId116"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F118" r:id="rId117"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F119" r:id="rId118"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-04 04:02:59 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1432,23 +1432,23 @@
         </is>
       </c>
       <c r="D33" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3412,23 +3412,23 @@
         </is>
       </c>
       <c r="D99" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3622,23 +3622,23 @@
         </is>
       </c>
       <c r="D106" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3802,23 +3802,23 @@
         </is>
       </c>
       <c r="D112" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4020,6 +4020,36 @@
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B120" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C120" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D120" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E120" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F120" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4145,6 +4175,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F117" r:id="rId116"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F118" r:id="rId117"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F119" r:id="rId118"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F120" r:id="rId119"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-05 04:01:46 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1462,23 +1462,23 @@
         </is>
       </c>
       <c r="D34" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3322,23 +3322,23 @@
         </is>
       </c>
       <c r="D96" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3442,23 +3442,23 @@
         </is>
       </c>
       <c r="D100" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3652,23 +3652,23 @@
         </is>
       </c>
       <c r="D107" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3832,23 +3832,23 @@
         </is>
       </c>
       <c r="D113" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4050,6 +4050,36 @@
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B121" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C121" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D121" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E121" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F121" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4176,6 +4206,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F118" r:id="rId117"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F119" r:id="rId118"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F120" r:id="rId119"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F121" r:id="rId120"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-06 03:52:05 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1492,23 +1492,23 @@
         </is>
       </c>
       <c r="D35" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3352,23 +3352,23 @@
         </is>
       </c>
       <c r="D97" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3472,23 +3472,23 @@
         </is>
       </c>
       <c r="D101" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3682,23 +3682,23 @@
         </is>
       </c>
       <c r="D108" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3862,23 +3862,23 @@
         </is>
       </c>
       <c r="D114" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4080,6 +4080,36 @@
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B122" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C122" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D122" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E122" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F122" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4207,6 +4237,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F119" r:id="rId118"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F120" r:id="rId119"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F121" r:id="rId120"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F122" r:id="rId121"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-07 04:08:10 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1522,23 +1522,23 @@
         </is>
       </c>
       <c r="D36" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3382,23 +3382,23 @@
         </is>
       </c>
       <c r="D98" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3502,23 +3502,23 @@
         </is>
       </c>
       <c r="D102" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3712,23 +3712,23 @@
         </is>
       </c>
       <c r="D109" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3892,23 +3892,23 @@
         </is>
       </c>
       <c r="D115" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4110,6 +4110,36 @@
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B123" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C123" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D123" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E123" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F123" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4238,6 +4268,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F120" r:id="rId119"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F121" r:id="rId120"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F122" r:id="rId121"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F123" r:id="rId122"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-08 04:06:04 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1552,23 +1552,23 @@
         </is>
       </c>
       <c r="D37" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3412,23 +3412,23 @@
         </is>
       </c>
       <c r="D99" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3532,23 +3532,23 @@
         </is>
       </c>
       <c r="D103" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3742,23 +3742,23 @@
         </is>
       </c>
       <c r="D110" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3922,23 +3922,23 @@
         </is>
       </c>
       <c r="D116" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4140,6 +4140,36 @@
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B124" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C124" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D124" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E124" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F124" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4269,6 +4299,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F121" r:id="rId120"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F122" r:id="rId121"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F123" r:id="rId122"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F124" r:id="rId123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-09 04:00:52 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1582,23 +1582,23 @@
         </is>
       </c>
       <c r="D38" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3442,23 +3442,23 @@
         </is>
       </c>
       <c r="D100" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3562,23 +3562,23 @@
         </is>
       </c>
       <c r="D104" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3772,23 +3772,23 @@
         </is>
       </c>
       <c r="D111" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3952,23 +3952,23 @@
         </is>
       </c>
       <c r="D117" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4170,6 +4170,36 @@
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B125" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C125" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D125" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E125" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F125" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4300,6 +4330,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F122" r:id="rId121"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F123" r:id="rId122"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F124" r:id="rId123"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F125" r:id="rId124"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-10 04:05:57 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1612,23 +1612,23 @@
         </is>
       </c>
       <c r="D39" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3472,23 +3472,23 @@
         </is>
       </c>
       <c r="D101" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3592,23 +3592,23 @@
         </is>
       </c>
       <c r="D105" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3802,23 +3802,23 @@
         </is>
       </c>
       <c r="D112" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3982,23 +3982,23 @@
         </is>
       </c>
       <c r="D118" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4200,6 +4200,36 @@
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B126" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C126" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D126" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E126" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F126" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4331,6 +4361,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F123" r:id="rId122"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F124" r:id="rId123"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F125" r:id="rId124"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F126" r:id="rId125"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-11 04:08:29 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1642,23 +1642,23 @@
         </is>
       </c>
       <c r="D40" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3502,23 +3502,23 @@
         </is>
       </c>
       <c r="D102" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3622,23 +3622,23 @@
         </is>
       </c>
       <c r="D106" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3832,23 +3832,23 @@
         </is>
       </c>
       <c r="D113" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4012,23 +4012,23 @@
         </is>
       </c>
       <c r="D119" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4230,6 +4230,36 @@
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B127" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C127" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D127" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E127" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F127" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4362,6 +4392,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F124" r:id="rId123"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F125" r:id="rId124"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F126" r:id="rId125"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F127" r:id="rId126"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-12 04:07:34 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1672,23 +1672,23 @@
         </is>
       </c>
       <c r="D41" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3532,23 +3532,23 @@
         </is>
       </c>
       <c r="D103" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3652,23 +3652,23 @@
         </is>
       </c>
       <c r="D107" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3862,23 +3862,23 @@
         </is>
       </c>
       <c r="D114" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4042,23 +4042,23 @@
         </is>
       </c>
       <c r="D120" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4260,6 +4260,36 @@
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B128" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C128" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D128" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E128" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F128" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4393,6 +4423,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F125" r:id="rId124"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F126" r:id="rId125"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F127" r:id="rId126"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F128" r:id="rId127"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-13 03:58:40 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1702,23 +1702,23 @@
         </is>
       </c>
       <c r="D42" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3562,23 +3562,23 @@
         </is>
       </c>
       <c r="D104" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E104" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F104" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3682,23 +3682,23 @@
         </is>
       </c>
       <c r="D108" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3892,23 +3892,23 @@
         </is>
       </c>
       <c r="D115" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4072,23 +4072,23 @@
         </is>
       </c>
       <c r="D121" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4290,6 +4290,36 @@
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B129" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C129" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D129" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E129" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F129" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4424,6 +4454,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F126" r:id="rId125"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F127" r:id="rId126"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F128" r:id="rId127"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F129" r:id="rId128"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-14 04:11:06 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1732,23 +1732,23 @@
         </is>
       </c>
       <c r="D43" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3592,23 +3592,23 @@
         </is>
       </c>
       <c r="D105" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E105" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F105" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3712,23 +3712,23 @@
         </is>
       </c>
       <c r="D109" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3922,23 +3922,23 @@
         </is>
       </c>
       <c r="D116" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4102,23 +4102,23 @@
         </is>
       </c>
       <c r="D122" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4320,6 +4320,36 @@
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B130" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C130" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D130" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E130" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F130" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4455,6 +4485,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F127" r:id="rId126"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F128" r:id="rId127"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F129" r:id="rId128"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F130" r:id="rId129"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-15 04:25:35 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1762,23 +1762,23 @@
         </is>
       </c>
       <c r="D44" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3622,23 +3622,23 @@
         </is>
       </c>
       <c r="D106" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F106" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3742,23 +3742,23 @@
         </is>
       </c>
       <c r="D110" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3952,23 +3952,23 @@
         </is>
       </c>
       <c r="D117" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4132,23 +4132,23 @@
         </is>
       </c>
       <c r="D123" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4350,6 +4350,36 @@
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B131" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C131" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D131" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E131" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F131" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4486,6 +4516,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F128" r:id="rId127"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F129" r:id="rId128"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F130" r:id="rId129"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F131" r:id="rId130"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-16 04:08:38 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1792,23 +1792,23 @@
         </is>
       </c>
       <c r="D45" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3652,23 +3652,23 @@
         </is>
       </c>
       <c r="D107" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E107" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F107" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3772,23 +3772,23 @@
         </is>
       </c>
       <c r="D111" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3982,23 +3982,23 @@
         </is>
       </c>
       <c r="D118" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4162,23 +4162,23 @@
         </is>
       </c>
       <c r="D124" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4380,6 +4380,36 @@
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B132" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C132" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D132" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E132" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F132" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4517,6 +4547,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F129" r:id="rId128"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F130" r:id="rId129"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F131" r:id="rId130"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F132" r:id="rId131"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-17 04:04:46 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1822,23 +1822,23 @@
         </is>
       </c>
       <c r="D46" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3682,23 +3682,23 @@
         </is>
       </c>
       <c r="D108" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E108" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F108" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3802,23 +3802,23 @@
         </is>
       </c>
       <c r="D112" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4012,23 +4012,23 @@
         </is>
       </c>
       <c r="D119" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4192,23 +4192,23 @@
         </is>
       </c>
       <c r="D125" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4410,6 +4410,36 @@
         </is>
       </c>
       <c r="F132" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B133" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C133" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D133" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E133" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F133" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4548,6 +4578,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F130" r:id="rId129"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F131" r:id="rId130"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F132" r:id="rId131"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F133" r:id="rId132"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-18 04:06:17 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1852,23 +1852,23 @@
         </is>
       </c>
       <c r="D47" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3712,23 +3712,23 @@
         </is>
       </c>
       <c r="D109" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E109" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F109" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3832,23 +3832,23 @@
         </is>
       </c>
       <c r="D113" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4042,23 +4042,23 @@
         </is>
       </c>
       <c r="D120" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4222,23 +4222,23 @@
         </is>
       </c>
       <c r="D126" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4440,6 +4440,36 @@
         </is>
       </c>
       <c r="F133" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B134" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C134" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D134" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E134" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F134" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4579,6 +4609,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F131" r:id="rId130"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F132" r:id="rId131"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F133" r:id="rId132"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F134" r:id="rId133"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-19 04:08:01 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1882,23 +1882,23 @@
         </is>
       </c>
       <c r="D48" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3742,23 +3742,23 @@
         </is>
       </c>
       <c r="D110" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E110" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F110" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3862,23 +3862,23 @@
         </is>
       </c>
       <c r="D114" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4072,23 +4072,23 @@
         </is>
       </c>
       <c r="D121" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4252,23 +4252,23 @@
         </is>
       </c>
       <c r="D127" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4470,6 +4470,36 @@
         </is>
       </c>
       <c r="F134" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B135" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C135" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D135" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E135" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F135" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4610,6 +4640,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F132" r:id="rId131"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F133" r:id="rId132"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F134" r:id="rId133"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F135" r:id="rId134"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-20 03:58:40 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1912,23 +1912,23 @@
         </is>
       </c>
       <c r="D49" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3772,23 +3772,23 @@
         </is>
       </c>
       <c r="D111" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E111" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F111" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3892,23 +3892,23 @@
         </is>
       </c>
       <c r="D115" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4102,23 +4102,23 @@
         </is>
       </c>
       <c r="D122" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4282,23 +4282,23 @@
         </is>
       </c>
       <c r="D128" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4500,6 +4500,36 @@
         </is>
       </c>
       <c r="F135" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B136" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C136" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D136" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E136" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F136" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4641,6 +4671,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F133" r:id="rId132"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F134" r:id="rId133"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F135" r:id="rId134"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F136" r:id="rId135"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-21 04:11:49 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1942,23 +1942,23 @@
         </is>
       </c>
       <c r="D50" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2422,23 +2422,23 @@
         </is>
       </c>
       <c r="D66" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2902,23 +2902,23 @@
         </is>
       </c>
       <c r="D82" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3322,23 +3322,23 @@
         </is>
       </c>
       <c r="D96" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3802,23 +3802,23 @@
         </is>
       </c>
       <c r="D112" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E112" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F112" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3922,23 +3922,23 @@
         </is>
       </c>
       <c r="D116" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4132,23 +4132,23 @@
         </is>
       </c>
       <c r="D123" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4312,23 +4312,23 @@
         </is>
       </c>
       <c r="D129" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4530,6 +4530,36 @@
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B137" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C137" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D137" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E137" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F137" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4672,6 +4702,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F134" r:id="rId133"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F135" r:id="rId134"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F136" r:id="rId135"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F137" r:id="rId136"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-22 04:25:36 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1972,23 +1972,23 @@
         </is>
       </c>
       <c r="D51" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2452,23 +2452,23 @@
         </is>
       </c>
       <c r="D67" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E67" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2932,23 +2932,23 @@
         </is>
       </c>
       <c r="D83" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E83" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3352,23 +3352,23 @@
         </is>
       </c>
       <c r="D97" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3832,23 +3832,23 @@
         </is>
       </c>
       <c r="D113" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E113" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F113" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3952,23 +3952,23 @@
         </is>
       </c>
       <c r="D117" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4162,23 +4162,23 @@
         </is>
       </c>
       <c r="D124" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E124" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F124" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4342,23 +4342,23 @@
         </is>
       </c>
       <c r="D130" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4560,6 +4560,36 @@
         </is>
       </c>
       <c r="F137" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B138" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C138" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D138" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E138" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F138" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4703,6 +4733,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F135" r:id="rId134"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F136" r:id="rId135"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F137" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F138" r:id="rId137"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-23 04:11:08 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>21-12-2025</t>
+          <t>22-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2002,23 +2002,23 @@
         </is>
       </c>
       <c r="D52" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2482,23 +2482,23 @@
         </is>
       </c>
       <c r="D68" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2962,23 +2962,23 @@
         </is>
       </c>
       <c r="D84" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3382,23 +3382,23 @@
         </is>
       </c>
       <c r="D98" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3862,23 +3862,23 @@
         </is>
       </c>
       <c r="D114" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E114" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F114" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3982,23 +3982,23 @@
         </is>
       </c>
       <c r="D118" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4192,23 +4192,23 @@
         </is>
       </c>
       <c r="D125" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E125" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F125" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4372,23 +4372,23 @@
         </is>
       </c>
       <c r="D131" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E131" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F131" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
@@ -4590,6 +4590,36 @@
         </is>
       </c>
       <c r="F138" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B139" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C139" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D139" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E139" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F139" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4734,6 +4764,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F136" r:id="rId135"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F137" r:id="rId136"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F138" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F139" r:id="rId138"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-24 04:08:37 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>22-12-2025</t>
+          <t>23-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>21-12-2025</t>
+          <t>22-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2032,23 +2032,23 @@
         </is>
       </c>
       <c r="D53" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E53" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2272,23 +2272,23 @@
         </is>
       </c>
       <c r="D61" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E61" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2512,23 +2512,23 @@
         </is>
       </c>
       <c r="D69" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E69" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2752,23 +2752,23 @@
         </is>
       </c>
       <c r="D77" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E77" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -2992,23 +2992,23 @@
         </is>
       </c>
       <c r="D85" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E85" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3172,23 +3172,23 @@
         </is>
       </c>
       <c r="D91" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E91" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3322,23 +3322,23 @@
         </is>
       </c>
       <c r="D96" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F96" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3412,23 +3412,23 @@
         </is>
       </c>
       <c r="D99" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3892,23 +3892,23 @@
         </is>
       </c>
       <c r="D115" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E115" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F115" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4012,23 +4012,23 @@
         </is>
       </c>
       <c r="D119" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4222,23 +4222,23 @@
         </is>
       </c>
       <c r="D126" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E126" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F126" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4402,23 +4402,23 @@
         </is>
       </c>
       <c r="D132" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E132" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F132" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -4620,6 +4620,36 @@
         </is>
       </c>
       <c r="F139" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B140" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C140" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D140" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E140" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F140" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4765,6 +4795,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F137" r:id="rId136"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F138" r:id="rId137"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F139" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F140" r:id="rId139"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-25 04:10:58 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>23-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>22-12-2025</t>
+          <t>23-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>21-12-2025</t>
+          <t>22-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2062,23 +2062,23 @@
         </is>
       </c>
       <c r="D54" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2302,23 +2302,23 @@
         </is>
       </c>
       <c r="D62" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2542,23 +2542,23 @@
         </is>
       </c>
       <c r="D70" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2782,23 +2782,23 @@
         </is>
       </c>
       <c r="D78" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="D86" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3202,23 +3202,23 @@
         </is>
       </c>
       <c r="D92" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3352,23 +3352,23 @@
         </is>
       </c>
       <c r="D97" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E97" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F97" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3442,23 +3442,23 @@
         </is>
       </c>
       <c r="D100" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3922,23 +3922,23 @@
         </is>
       </c>
       <c r="D116" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E116" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F116" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4042,23 +4042,23 @@
         </is>
       </c>
       <c r="D120" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E120" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F120" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4252,23 +4252,23 @@
         </is>
       </c>
       <c r="D127" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E127" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F127" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4432,23 +4432,23 @@
         </is>
       </c>
       <c r="D133" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E133" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F133" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -4628,7 +4628,7 @@
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -4650,6 +4650,36 @@
         </is>
       </c>
       <c r="F140" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B141" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C141" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D141" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E141" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F141" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4796,6 +4826,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F138" r:id="rId137"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F139" r:id="rId138"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F140" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F141" r:id="rId140"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-26 04:08:36 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>24-12-2025</t>
+          <t>25-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>23-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>22-12-2025</t>
+          <t>23-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>21-12-2025</t>
+          <t>22-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2092,23 +2092,23 @@
         </is>
       </c>
       <c r="D55" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E55" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2332,23 +2332,23 @@
         </is>
       </c>
       <c r="D63" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E63" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2572,23 +2572,23 @@
         </is>
       </c>
       <c r="D71" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E71" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2662,23 +2662,23 @@
         </is>
       </c>
       <c r="D74" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2812,23 +2812,23 @@
         </is>
       </c>
       <c r="D79" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E79" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3052,23 +3052,23 @@
         </is>
       </c>
       <c r="D87" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E87" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3128,7 +3128,7 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3232,23 +3232,23 @@
         </is>
       </c>
       <c r="D93" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E93" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3382,23 +3382,23 @@
         </is>
       </c>
       <c r="D98" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F98" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3472,23 +3472,23 @@
         </is>
       </c>
       <c r="D101" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E101" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F101" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3952,23 +3952,23 @@
         </is>
       </c>
       <c r="D117" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E117" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F117" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4072,23 +4072,23 @@
         </is>
       </c>
       <c r="D121" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E121" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F121" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4282,23 +4282,23 @@
         </is>
       </c>
       <c r="D128" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E128" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F128" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4462,23 +4462,23 @@
         </is>
       </c>
       <c r="D134" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E134" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F134" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -4628,7 +4628,7 @@
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -4658,7 +4658,7 @@
     <row r="141">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -4680,6 +4680,36 @@
         </is>
       </c>
       <c r="F141" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B142" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C142" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D142" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E142" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F142" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4827,6 +4857,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F139" r:id="rId138"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F140" r:id="rId139"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F141" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F142" r:id="rId141"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-27 04:06:10 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>25-12-2025</t>
+          <t>26-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>24-12-2025</t>
+          <t>25-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>23-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>22-12-2025</t>
+          <t>23-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>21-12-2025</t>
+          <t>22-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2122,23 +2122,23 @@
         </is>
       </c>
       <c r="D56" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2212,23 +2212,23 @@
         </is>
       </c>
       <c r="D59" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E59" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2362,23 +2362,23 @@
         </is>
       </c>
       <c r="D64" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2602,23 +2602,23 @@
         </is>
       </c>
       <c r="D72" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2692,23 +2692,23 @@
         </is>
       </c>
       <c r="D75" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E75" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2738,7 +2738,7 @@
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2842,23 +2842,23 @@
         </is>
       </c>
       <c r="D80" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2888,7 +2888,7 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3082,23 +3082,23 @@
         </is>
       </c>
       <c r="D88" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3158,7 +3158,7 @@
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3262,23 +3262,23 @@
         </is>
       </c>
       <c r="D94" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F94" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3308,7 +3308,7 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3412,23 +3412,23 @@
         </is>
       </c>
       <c r="D99" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E99" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F99" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3502,23 +3502,23 @@
         </is>
       </c>
       <c r="D102" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F102" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3548,7 +3548,7 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3982,23 +3982,23 @@
         </is>
       </c>
       <c r="D118" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E118" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F118" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4028,7 +4028,7 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4102,23 +4102,23 @@
         </is>
       </c>
       <c r="D122" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E122" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F122" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4148,7 +4148,7 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4312,23 +4312,23 @@
         </is>
       </c>
       <c r="D129" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E129" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F129" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4358,7 +4358,7 @@
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4492,23 +4492,23 @@
         </is>
       </c>
       <c r="D135" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E135" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F135" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4538,7 +4538,7 @@
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -4628,7 +4628,7 @@
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -4658,7 +4658,7 @@
     <row r="141">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -4688,7 +4688,7 @@
     <row r="142">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -4710,6 +4710,36 @@
         </is>
       </c>
       <c r="F142" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B143" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C143" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D143" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E143" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F143" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4858,6 +4888,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F140" r:id="rId139"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F141" r:id="rId140"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F142" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F143" r:id="rId142"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Nalco data (2025-12-28 04:29:43 UTC)
</commit_message>
<xml_diff>
--- a/data/nalco_prices.xlsx
+++ b/data/nalco_prices.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -488,7 +488,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>26-12-2025</t>
+          <t>27-12-2025</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>25-12-2025</t>
+          <t>26-12-2025</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
@@ -548,7 +548,7 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>24-12-2025</t>
+          <t>25-12-2025</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>23-12-2025</t>
+          <t>24-12-2025</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
@@ -608,7 +608,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>22-12-2025</t>
+          <t>23-12-2025</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>21-12-2025</t>
+          <t>22-12-2025</t>
         </is>
       </c>
       <c r="B7" s="3" t="inlineStr">
@@ -668,7 +668,7 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>20-12-2025</t>
+          <t>21-12-2025</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
         <is>
-          <t>19-12-2025</t>
+          <t>20-12-2025</t>
         </is>
       </c>
       <c r="B9" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>18-12-2025</t>
+          <t>19-12-2025</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
@@ -758,7 +758,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>17-12-2025</t>
+          <t>18-12-2025</t>
         </is>
       </c>
       <c r="B11" s="3" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>16-12-2025</t>
+          <t>17-12-2025</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>15-12-2025</t>
+          <t>16-12-2025</t>
         </is>
       </c>
       <c r="B13" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>14-12-2025</t>
+          <t>15-12-2025</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>13-12-2025</t>
+          <t>14-12-2025</t>
         </is>
       </c>
       <c r="B15" s="3" t="inlineStr">
@@ -908,7 +908,7 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>12-12-2025</t>
+          <t>13-12-2025</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
@@ -938,7 +938,7 @@
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>11-12-2025</t>
+          <t>12-12-2025</t>
         </is>
       </c>
       <c r="B17" s="3" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>10-12-2025</t>
+          <t>11-12-2025</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -998,7 +998,7 @@
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>09-12-2025</t>
+          <t>10-12-2025</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>08-12-2025</t>
+          <t>09-12-2025</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>07-12-2025</t>
+          <t>08-12-2025</t>
         </is>
       </c>
       <c r="B21" s="3" t="inlineStr">
@@ -1088,7 +1088,7 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>06-12-2025</t>
+          <t>07-12-2025</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>05-12-2025</t>
+          <t>06-12-2025</t>
         </is>
       </c>
       <c r="B23" s="3" t="inlineStr">
@@ -1148,7 +1148,7 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>04-12-2025</t>
+          <t>05-12-2025</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
@@ -1178,7 +1178,7 @@
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>03-12-2025</t>
+          <t>04-12-2025</t>
         </is>
       </c>
       <c r="B25" s="3" t="inlineStr">
@@ -1208,7 +1208,7 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>02-12-2025</t>
+          <t>03-12-2025</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
@@ -1238,7 +1238,7 @@
     <row r="27">
       <c r="A27" s="3" t="inlineStr">
         <is>
-          <t>01-12-2025</t>
+          <t>02-12-2025</t>
         </is>
       </c>
       <c r="B27" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>30-11-2025</t>
+          <t>01-12-2025</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
@@ -1298,7 +1298,7 @@
     <row r="29">
       <c r="A29" s="3" t="inlineStr">
         <is>
-          <t>29-11-2025</t>
+          <t>30-11-2025</t>
         </is>
       </c>
       <c r="B29" s="3" t="inlineStr">
@@ -1328,7 +1328,7 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>28-11-2025</t>
+          <t>29-11-2025</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
@@ -1358,7 +1358,7 @@
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="B31" s="3" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
@@ -1418,7 +1418,7 @@
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="B33" s="3" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>23-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="B35" s="3" t="inlineStr">
@@ -1508,7 +1508,7 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>22-11-2025</t>
+          <t>23-11-2025</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
@@ -1538,7 +1538,7 @@
     <row r="37">
       <c r="A37" s="3" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>22-11-2025</t>
         </is>
       </c>
       <c r="B37" s="3" t="inlineStr">
@@ -1568,7 +1568,7 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
@@ -1598,7 +1598,7 @@
     <row r="39">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>19-11-2025</t>
+          <t>20-11-2025</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>18-11-2025</t>
+          <t>19-11-2025</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
@@ -1658,7 +1658,7 @@
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>17-11-2025</t>
+          <t>18-11-2025</t>
         </is>
       </c>
       <c r="B41" s="3" t="inlineStr">
@@ -1688,7 +1688,7 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>16-11-2025</t>
+          <t>17-11-2025</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>15-11-2025</t>
+          <t>16-11-2025</t>
         </is>
       </c>
       <c r="B43" s="3" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>14-11-2025</t>
+          <t>15-11-2025</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
@@ -1778,7 +1778,7 @@
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>13-11-2025</t>
+          <t>14-11-2025</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
@@ -1808,7 +1808,7 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>12-11-2025</t>
+          <t>13-11-2025</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
@@ -1838,7 +1838,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>11-11-2025</t>
+          <t>12-11-2025</t>
         </is>
       </c>
       <c r="B47" s="3" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>10-11-2025</t>
+          <t>11-11-2025</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>09-11-2025</t>
+          <t>10-11-2025</t>
         </is>
       </c>
       <c r="B49" s="3" t="inlineStr">
@@ -1928,7 +1928,7 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>08-11-2025</t>
+          <t>09-11-2025</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>07-11-2025</t>
+          <t>08-11-2025</t>
         </is>
       </c>
       <c r="B51" s="3" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>06-11-2025</t>
+          <t>07-11-2025</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>05-11-2025</t>
+          <t>06-11-2025</t>
         </is>
       </c>
       <c r="B53" s="3" t="inlineStr">
@@ -2048,7 +2048,7 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>04-11-2025</t>
+          <t>05-11-2025</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
@@ -2078,7 +2078,7 @@
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>03-11-2025</t>
+          <t>04-11-2025</t>
         </is>
       </c>
       <c r="B55" s="3" t="inlineStr">
@@ -2108,7 +2108,7 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>02-11-2025</t>
+          <t>03-11-2025</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="B57" s="3" t="inlineStr">
@@ -2152,23 +2152,23 @@
         </is>
       </c>
       <c r="D57" s="4" t="n">
-        <v>297.15</v>
+        <v>296.05</v>
       </c>
       <c r="E57" s="3" t="inlineStr">
         <is>
-          <t>01-11-2025</t>
+          <t>02-11-2025</t>
         </is>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-02-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>31-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
@@ -2182,23 +2182,23 @@
         </is>
       </c>
       <c r="D58" s="4" t="n">
-        <v>294.05</v>
+        <v>297.15</v>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>01-11-2025</t>
         </is>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-11-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>30-10-2025</t>
+          <t>31-10-2025</t>
         </is>
       </c>
       <c r="B59" s="3" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
@@ -2242,23 +2242,23 @@
         </is>
       </c>
       <c r="D60" s="4" t="n">
-        <v>288.55</v>
+        <v>294.05</v>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>30-10-2025</t>
         </is>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-30-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>28-10-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="B61" s="3" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>27-10-2025</t>
+          <t>28-10-2025</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>26-10-2025</t>
+          <t>27-10-2025</t>
         </is>
       </c>
       <c r="B63" s="3" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>25-10-2025</t>
+          <t>26-10-2025</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>24-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
@@ -2392,23 +2392,23 @@
         </is>
       </c>
       <c r="D65" s="4" t="n">
-        <v>282.45</v>
+        <v>288.55</v>
       </c>
       <c r="E65" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>25-10-2025</t>
         </is>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-25-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>23-10-2025</t>
+          <t>24-10-2025</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>22-10-2025</t>
+          <t>23-10-2025</t>
         </is>
       </c>
       <c r="B67" s="3" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>21-10-2025</t>
+          <t>22-10-2025</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>20-10-2025</t>
+          <t>21-10-2025</t>
         </is>
       </c>
       <c r="B69" s="3" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>19-10-2025</t>
+          <t>20-10-2025</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>18-10-2025</t>
+          <t>19-10-2025</t>
         </is>
       </c>
       <c r="B71" s="3" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>17-10-2025</t>
+          <t>18-10-2025</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>16-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="B73" s="3" t="inlineStr">
@@ -2632,23 +2632,23 @@
         </is>
       </c>
       <c r="D73" s="4" t="n">
-        <v>285.05</v>
+        <v>282.45</v>
       </c>
       <c r="E73" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>17-10-2025</t>
         </is>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-17-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>15-10-2025</t>
+          <t>16-10-2025</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>14-10-2025</t>
+          <t>15-10-2025</t>
         </is>
       </c>
       <c r="B75" s="3" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>13-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
@@ -2722,23 +2722,23 @@
         </is>
       </c>
       <c r="D76" s="4" t="n">
-        <v>282.85</v>
+        <v>285.05</v>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>14-10-2025</t>
         </is>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-14-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>12-10-2025</t>
+          <t>13-10-2025</t>
         </is>
       </c>
       <c r="B77" s="3" t="inlineStr">
@@ -2768,7 +2768,7 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>11-10-2025</t>
+          <t>12-10-2025</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
@@ -2798,7 +2798,7 @@
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>10-10-2025</t>
+          <t>11-10-2025</t>
         </is>
       </c>
       <c r="B79" s="3" t="inlineStr">
@@ -2828,7 +2828,7 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>09-10-2025</t>
+          <t>10-10-2025</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>08-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="B81" s="3" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="D81" s="4" t="n">
-        <v>277.95</v>
+        <v>282.85</v>
       </c>
       <c r="E81" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>09-10-2025</t>
         </is>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-09-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>07-10-2025</t>
+          <t>08-10-2025</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>06-10-2025</t>
+          <t>07-10-2025</t>
         </is>
       </c>
       <c r="B83" s="3" t="inlineStr">
@@ -2948,7 +2948,7 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>05-10-2025</t>
+          <t>06-10-2025</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
@@ -2978,7 +2978,7 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>04-10-2025</t>
+          <t>05-10-2025</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
@@ -3008,7 +3008,7 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>03-10-2025</t>
+          <t>04-10-2025</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
@@ -3038,7 +3038,7 @@
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>02-10-2025</t>
+          <t>03-10-2025</t>
         </is>
       </c>
       <c r="B87" s="3" t="inlineStr">
@@ -3068,7 +3068,7 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>01-10-2025</t>
+          <t>02-10-2025</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
@@ -3098,7 +3098,7 @@
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="B89" s="3" t="inlineStr">
@@ -3112,23 +3112,23 @@
         </is>
       </c>
       <c r="D89" s="4" t="n">
-        <v>274.95</v>
+        <v>277.95</v>
       </c>
       <c r="E89" s="3" t="inlineStr">
         <is>
-          <t>30-09-2025</t>
+          <t>01-10-2025</t>
         </is>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-01-10-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
@@ -3142,23 +3142,23 @@
         </is>
       </c>
       <c r="D90" s="4" t="n">
-        <v>270.25</v>
+        <v>274.95</v>
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>30-09-2025</t>
         </is>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/09/INGOT-30-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>28-09-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="B91" s="3" t="inlineStr">
@@ -3188,7 +3188,7 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>27-09-2025</t>
+          <t>28-09-2025</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>26-09-2025</t>
+          <t>27-09-2025</t>
         </is>
       </c>
       <c r="B93" s="3" t="inlineStr">
@@ -3248,7 +3248,7 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>25-09-2025</t>
+          <t>26-09-2025</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
@@ -3278,7 +3278,7 @@
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>24-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="B95" s="3" t="inlineStr">
@@ -3292,23 +3292,23 @@
         </is>
       </c>
       <c r="D95" s="4" t="n">
-        <v>275.25</v>
+        <v>270.25</v>
       </c>
       <c r="E95" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>25-09-2025</t>
         </is>
       </c>
       <c r="F95" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-25-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>23-09-2025</t>
+          <t>24-09-2025</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
@@ -3338,7 +3338,7 @@
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>22-09-2025</t>
+          <t>23-09-2025</t>
         </is>
       </c>
       <c r="B97" s="3" t="inlineStr">
@@ -3368,7 +3368,7 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>21-09-2025</t>
+          <t>22-09-2025</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
@@ -3398,7 +3398,7 @@
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>20-09-2025</t>
+          <t>21-09-2025</t>
         </is>
       </c>
       <c r="B99" s="3" t="inlineStr">
@@ -3428,7 +3428,7 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>19-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
@@ -3442,23 +3442,23 @@
         </is>
       </c>
       <c r="D100" s="4" t="n">
-        <v>278.95</v>
+        <v>275.25</v>
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>20-09-2025</t>
         </is>
       </c>
       <c r="F100" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-20-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>18-09-2025</t>
+          <t>19-09-2025</t>
         </is>
       </c>
       <c r="B101" s="3" t="inlineStr">
@@ -3488,7 +3488,7 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>17-09-2025</t>
+          <t>18-09-2025</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
@@ -3518,7 +3518,7 @@
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>16-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="B103" s="3" t="inlineStr">
@@ -3532,23 +3532,23 @@
         </is>
       </c>
       <c r="D103" s="4" t="n">
-        <v>272.05</v>
+        <v>278.95</v>
       </c>
       <c r="E103" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>17-09-2025</t>
         </is>
       </c>
       <c r="F103" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-17-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>15-09-2025</t>
+          <t>16-09-2025</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>14-09-2025</t>
+          <t>15-09-2025</t>
         </is>
       </c>
       <c r="B105" s="3" t="inlineStr">
@@ -3608,7 +3608,7 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>13-09-2025</t>
+          <t>14-09-2025</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
@@ -3638,7 +3638,7 @@
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>12-09-2025</t>
+          <t>13-09-2025</t>
         </is>
       </c>
       <c r="B107" s="3" t="inlineStr">
@@ -3668,7 +3668,7 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>11-09-2025</t>
+          <t>12-09-2025</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>10-09-2025</t>
+          <t>11-09-2025</t>
         </is>
       </c>
       <c r="B109" s="3" t="inlineStr">
@@ -3728,7 +3728,7 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>09-09-2025</t>
+          <t>10-09-2025</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
@@ -3758,7 +3758,7 @@
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>08-09-2025</t>
+          <t>09-09-2025</t>
         </is>
       </c>
       <c r="B111" s="3" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>07-09-2025</t>
+          <t>08-09-2025</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
@@ -3818,7 +3818,7 @@
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>06-09-2025</t>
+          <t>07-09-2025</t>
         </is>
       </c>
       <c r="B113" s="3" t="inlineStr">
@@ -3848,7 +3848,7 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>05-09-2025</t>
+          <t>06-09-2025</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
@@ -3878,7 +3878,7 @@
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>04-09-2025</t>
+          <t>05-09-2025</t>
         </is>
       </c>
       <c r="B115" s="3" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>03-09-2025</t>
+          <t>04-09-2025</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>02-09-2025</t>
+          <t>03-09-2025</t>
         </is>
       </c>
       <c r="B117" s="3" t="inlineStr">
@@ -3968,7 +3968,7 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>01-09-2025</t>
+          <t>02-09-2025</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
@@ -3998,7 +3998,7 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>31-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="B119" s="3" t="inlineStr">
@@ -4012,23 +4012,23 @@
         </is>
       </c>
       <c r="D119" s="4" t="n">
-        <v>271.05</v>
+        <v>272.05</v>
       </c>
       <c r="E119" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>01-09-2025</t>
         </is>
       </c>
       <c r="F119" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-01-09-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>30-08-2025</t>
+          <t>31-08-2025</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
@@ -4058,7 +4058,7 @@
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>29-08-2025</t>
+          <t>30-08-2025</t>
         </is>
       </c>
       <c r="B121" s="3" t="inlineStr">
@@ -4088,7 +4088,7 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>28-08-2025</t>
+          <t>29-08-2025</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
@@ -4118,7 +4118,7 @@
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>27-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="B123" s="3" t="inlineStr">
@@ -4132,23 +4132,23 @@
         </is>
       </c>
       <c r="D123" s="4" t="n">
-        <v>264.35</v>
+        <v>271.05</v>
       </c>
       <c r="E123" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>28-08-2025</t>
         </is>
       </c>
       <c r="F123" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-28-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>26-08-2025</t>
+          <t>27-08-2025</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
@@ -4178,7 +4178,7 @@
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>25-08-2025</t>
+          <t>26-08-2025</t>
         </is>
       </c>
       <c r="B125" s="3" t="inlineStr">
@@ -4208,7 +4208,7 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>24-08-2025</t>
+          <t>25-08-2025</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
@@ -4238,7 +4238,7 @@
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>23-08-2025</t>
+          <t>24-08-2025</t>
         </is>
       </c>
       <c r="B127" s="3" t="inlineStr">
@@ -4268,7 +4268,7 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>22-08-2025</t>
+          <t>23-08-2025</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>21-08-2025</t>
+          <t>22-08-2025</t>
         </is>
       </c>
       <c r="B129" s="3" t="inlineStr">
@@ -4328,7 +4328,7 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>20-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
@@ -4342,23 +4342,23 @@
         </is>
       </c>
       <c r="D130" s="4" t="n">
-        <v>269.45</v>
+        <v>264.35</v>
       </c>
       <c r="E130" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>21-08-2025</t>
         </is>
       </c>
       <c r="F130" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/INGOT-21-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>19-08-2025</t>
+          <t>20-08-2025</t>
         </is>
       </c>
       <c r="B131" s="3" t="inlineStr">
@@ -4388,7 +4388,7 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>18-08-2025</t>
+          <t>19-08-2025</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
@@ -4418,7 +4418,7 @@
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>17-08-2025</t>
+          <t>18-08-2025</t>
         </is>
       </c>
       <c r="B133" s="3" t="inlineStr">
@@ -4448,7 +4448,7 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>16-08-2025</t>
+          <t>17-08-2025</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
@@ -4478,7 +4478,7 @@
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>15-08-2025</t>
+          <t>16-08-2025</t>
         </is>
       </c>
       <c r="B135" s="3" t="inlineStr">
@@ -4508,7 +4508,7 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>14-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
@@ -4522,23 +4522,23 @@
         </is>
       </c>
       <c r="D136" s="4" t="n">
-        <v>268.25</v>
+        <v>269.45</v>
       </c>
       <c r="E136" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>15-08-2025</t>
         </is>
       </c>
       <c r="F136" s="3" t="inlineStr">
         <is>
-          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+          <t>https://nalcoindia.com/wp-content/uploads/2025/08/INGOT-15-08-2025.pdf</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>13-08-2025</t>
+          <t>14-08-2025</t>
         </is>
       </c>
       <c r="B137" s="3" t="inlineStr">
@@ -4568,7 +4568,7 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>12-08-2025</t>
+          <t>13-08-2025</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
@@ -4598,7 +4598,7 @@
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>11-08-2025</t>
+          <t>12-08-2025</t>
         </is>
       </c>
       <c r="B139" s="3" t="inlineStr">
@@ -4628,7 +4628,7 @@
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>10-08-2025</t>
+          <t>11-08-2025</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
@@ -4658,7 +4658,7 @@
     <row r="141">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>09-08-2025</t>
+          <t>10-08-2025</t>
         </is>
       </c>
       <c r="B141" s="3" t="inlineStr">
@@ -4688,7 +4688,7 @@
     <row r="142">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>08-08-2025</t>
+          <t>09-08-2025</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
@@ -4718,7 +4718,7 @@
     <row r="143">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>07-08-2025</t>
+          <t>08-08-2025</t>
         </is>
       </c>
       <c r="B143" s="3" t="inlineStr">
@@ -4740,6 +4740,36 @@
         </is>
       </c>
       <c r="F143" s="3" t="inlineStr">
+        <is>
+          <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="B144" s="3" t="inlineStr">
+        <is>
+          <t>ALUMINIUM INGOT</t>
+        </is>
+      </c>
+      <c r="C144" s="3" t="inlineStr">
+        <is>
+          <t>IE07</t>
+        </is>
+      </c>
+      <c r="D144" s="4" t="n">
+        <v>268.25</v>
+      </c>
+      <c r="E144" s="3" t="inlineStr">
+        <is>
+          <t>07-08-2025</t>
+        </is>
+      </c>
+      <c r="F144" s="3" t="inlineStr">
         <is>
           <t>https://nalcoindia.com/wp-content/uploads/2019/01/Ingot-07-08-2025.pdf</t>
         </is>
@@ -4889,6 +4919,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F141" r:id="rId140"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F142" r:id="rId141"/>
   